<commit_message>
schedule builder working except for sunrise/sunset offset time reference
</commit_message>
<xml_diff>
--- a/data/sample_input/TimeScheduleConfig.xlsx
+++ b/data/sample_input/TimeScheduleConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sesa368046\src\astroscheduler\data\sample_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AD7DFAF-F16F-4F0B-A033-C984210483B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55CE325-5ACD-4E45-B18F-A19F55C8EC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{27BC9DC3-E900-43F2-B8D0-6E87A6A1ECD7}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{27BC9DC3-E900-43F2-B8D0-6E87A6A1ECD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entries" sheetId="1" r:id="rId1"/>
@@ -96,9 +96,6 @@
     <t>EBOVersion</t>
   </si>
   <si>
-    <t>6.0.4.90</t>
-  </si>
-  <si>
     <t>ReferenceYear</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>TimeReference Absolute means the entry starts at the time of day Hour:Minute</t>
+  </si>
+  <si>
+    <t>5.0.3.117</t>
   </si>
 </sst>
 </file>
@@ -465,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F97FC5B-F882-4C6F-87FD-9B1B24A8C071}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -493,7 +493,7 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -513,7 +513,7 @@
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -533,7 +533,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -570,7 +570,7 @@
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -602,8 +602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118592A6-78D1-4381-B65B-E6106D87DE35}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +646,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5">
         <f ca="1">YEAR(TODAY())</f>
@@ -658,7 +658,7 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -670,6 +670,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="70b5b486-62ca-446d-85b9-12534f89bcbd" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c56cb509-70af-4579-bdf7-5ea3b144dfb6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100249B0E9FE56F5948B602BA84FE20E907" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63949f8d055d5943d96d237c4ef691d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c56cb509-70af-4579-bdf7-5ea3b144dfb6" xmlns:ns3="70b5b486-62ca-446d-85b9-12534f89bcbd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb804e7b5fa037c4b3c9872285b34489" ns2:_="" ns3:_="">
     <xsd:import namespace="c56cb509-70af-4579-bdf7-5ea3b144dfb6"/>
@@ -904,27 +924,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="70b5b486-62ca-446d-85b9-12534f89bcbd" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c56cb509-70af-4579-bdf7-5ea3b144dfb6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7E3410-FB96-4A4F-BEF0-80AF9C94BD2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="70b5b486-62ca-446d-85b9-12534f89bcbd"/>
+    <ds:schemaRef ds:uri="c56cb509-70af-4579-bdf7-5ea3b144dfb6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E8BA42F-44F7-436B-8FF8-451BF8769D27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D302D409-78E5-462F-B93A-F03EF0CB1A60}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -943,25 +962,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E8BA42F-44F7-436B-8FF8-451BF8769D27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7E3410-FB96-4A4F-BEF0-80AF9C94BD2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="70b5b486-62ca-446d-85b9-12534f89bcbd"/>
-    <ds:schemaRef ds:uri="c56cb509-70af-4579-bdf7-5ea3b144dfb6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{57443d00-af18-408c-9335-47b5de3ec9b9}" enabled="1" method="Privileged" siteId="{6e51e1ad-c54b-4b39-b598-0ffe9ae68fef}" contentBits="2" removed="0"/>

</xml_diff>

<commit_message>
astronical schedule builder working but in need of doctrings, README and error catching
</commit_message>
<xml_diff>
--- a/data/sample_input/TimeScheduleConfig.xlsx
+++ b/data/sample_input/TimeScheduleConfig.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sesa368046\src\astroscheduler\data\sample_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55CE325-5ACD-4E45-B18F-A19F55C8EC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C3D3FC-7324-4813-8B9F-431F08BC5D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{27BC9DC3-E900-43F2-B8D0-6E87A6A1ECD7}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{27BC9DC3-E900-43F2-B8D0-6E87A6A1ECD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entries" sheetId="1" r:id="rId1"/>
@@ -465,8 +465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F97FC5B-F882-4C6F-87FD-9B1B24A8C071}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -602,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{118592A6-78D1-4381-B65B-E6106D87DE35}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -670,26 +670,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="70b5b486-62ca-446d-85b9-12534f89bcbd" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c56cb509-70af-4579-bdf7-5ea3b144dfb6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100249B0E9FE56F5948B602BA84FE20E907" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63949f8d055d5943d96d237c4ef691d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c56cb509-70af-4579-bdf7-5ea3b144dfb6" xmlns:ns3="70b5b486-62ca-446d-85b9-12534f89bcbd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fb804e7b5fa037c4b3c9872285b34489" ns2:_="" ns3:_="">
     <xsd:import namespace="c56cb509-70af-4579-bdf7-5ea3b144dfb6"/>
@@ -924,26 +904,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="70b5b486-62ca-446d-85b9-12534f89bcbd" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c56cb509-70af-4579-bdf7-5ea3b144dfb6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7E3410-FB96-4A4F-BEF0-80AF9C94BD2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="70b5b486-62ca-446d-85b9-12534f89bcbd"/>
-    <ds:schemaRef ds:uri="c56cb509-70af-4579-bdf7-5ea3b144dfb6"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E8BA42F-44F7-436B-8FF8-451BF8769D27}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D302D409-78E5-462F-B93A-F03EF0CB1A60}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -962,6 +943,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E8BA42F-44F7-436B-8FF8-451BF8769D27}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE7E3410-FB96-4A4F-BEF0-80AF9C94BD2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="70b5b486-62ca-446d-85b9-12534f89bcbd"/>
+    <ds:schemaRef ds:uri="c56cb509-70af-4579-bdf7-5ea3b144dfb6"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{57443d00-af18-408c-9335-47b5de3ec9b9}" enabled="1" method="Privileged" siteId="{6e51e1ad-c54b-4b39-b598-0ffe9ae68fef}" contentBits="2" removed="0"/>

</xml_diff>